<commit_message>
14_Aug_2020 => added Class new Create_GoogleMaps_Link->createLink() both to getCoordsListFromSlaveExcel.php and proccess_main_via_ajax.php
</commit_message>
<xml_diff>
--- a/Geocoding_Process_Module/Slave_data.xlsx
+++ b/Geocoding_Process_Module/Slave_data.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Trelle Ager 11 Syddanmark </t>
   </si>
@@ -33,6 +33,24 @@
   </si>
   <si>
     <t>10.39632, 55.398591</t>
+  </si>
+  <si>
+    <t>Frederiksborgvej 13-5  </t>
+  </si>
+  <si>
+    <t>12.531159, 55.71852</t>
+  </si>
+  <si>
+    <t>Buddingevej 66  </t>
+  </si>
+  <si>
+    <t>12.495893, 55.762853</t>
+  </si>
+  <si>
+    <t>Ny Kronborgvej 2  </t>
+  </si>
+  <si>
+    <t>12.614004, 56.039332</t>
   </si>
 </sst>
 </file>
@@ -83,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <cols>
     <col min="1" max="1" width="28"/>
     <col min="2" max="2" width="21"/>
@@ -121,6 +139,30 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>